<commit_message>
1. TileMapTool Window 추가 생성 2. TileMapToolScene 설계 3. TileMapRenderer 클래스 설계 4. Tile 클래스 설계
</commit_message>
<xml_diff>
--- a/스타듀밸리_Win32API_김다인_Contents&Function.xlsx
+++ b/스타듀밸리_Win32API_김다인_Contents&Function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StardewVelly_InnyEngine_Win32API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325621D0-1F55-4928-9C60-8B8C16741818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4159335-1224-48ED-9DC3-F800323B7D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DAD171CC-0285-4BF8-BECE-3F60597F3648}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DAD171CC-0285-4BF8-BECE-3F60597F3648}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
   <si>
     <t>Player</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -384,6 +384,9 @@
   <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Progress </t>
   </si>
 </sst>
 </file>
@@ -481,7 +484,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -506,7 +509,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -514,15 +517,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E32B991-2ACC-47FF-BF94-29DC9CD2AFBC}">
   <dimension ref="B1:I29"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -878,9 +872,7 @@
       <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="2:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="9">
@@ -894,9 +886,6 @@
         <v>14</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="6" spans="2:9" ht="104.4" x14ac:dyDescent="0.4">
       <c r="B6" s="9">
@@ -939,7 +928,9 @@
       <c r="E8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B9" s="9">
@@ -1067,7 +1058,9 @@
         <v>0</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B19" s="9">
@@ -1096,23 +1089,23 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B21" s="11">
+      <c r="B21" s="9">
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B22" s="11">
+      <c r="B22" s="9">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="5"/>
@@ -1120,10 +1113,10 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B23" s="11">
+      <c r="B23" s="9">
         <v>19</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D23" s="5"/>
@@ -1131,10 +1124,10 @@
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <v>20</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="5"/>
@@ -1145,7 +1138,7 @@
       <c r="B25" s="1">
         <v>21</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1158,7 +1151,7 @@
       <c r="B26" s="1">
         <v>22</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -1171,7 +1164,7 @@
       <c r="B27" s="1">
         <v>23</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -1184,7 +1177,7 @@
       <c r="B28" s="1">
         <v>24</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
@@ -1197,7 +1190,7 @@
       <c r="B29" s="1">
         <v>25</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1208,6 +1201,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F29" xr:uid="{D0A3525D-AD1D-4461-89A3-03694DAB6710}">
+      <formula1>"Complete, Progress "</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1217,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D785CD-CB04-4040-B65C-5CBC572542AE}">
   <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1492,7 +1490,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B21" s="11">
+      <c r="B21" s="9">
         <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1505,10 +1503,10 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B22" s="11">
+      <c r="B22" s="9">
         <v>18</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -1520,26 +1518,26 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B23" s="11">
+      <c r="B23" s="9">
         <v>19</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <v>20</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="1" t="s">
         <v>71</v>
       </c>
       <c r="E24" s="2"/>
@@ -1567,7 +1565,7 @@
       <c r="C26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E26" s="2"/>
@@ -1595,7 +1593,7 @@
       <c r="C28" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="2"/>
@@ -1623,7 +1621,7 @@
       <c r="C30" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E30" s="2"/>
@@ -1652,7 +1650,7 @@
       <c r="D32" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F32" s="1"/>

</xml_diff>

<commit_message>
1. Collision Enter, Stay, Exit 함수 구현 2. FarmScene 내 Object 수정
</commit_message>
<xml_diff>
--- a/스타듀밸리_Win32API_김다인_Contents&Function.xlsx
+++ b/스타듀밸리_Win32API_김다인_Contents&Function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StardewVelly_InnyEngine_Win32API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4159335-1224-48ED-9DC3-F800323B7D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41E8236-0E26-48FE-B492-CB194B577BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DAD171CC-0285-4BF8-BECE-3F60597F3648}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DAD171CC-0285-4BF8-BECE-3F60597F3648}"/>
   </bookViews>
   <sheets>
     <sheet name="Common" sheetId="7" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Common!$C$4:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Scene!$D$4:$E$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Common!$A$1:$G$30</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Scene!$A$1:$G$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Scene!$A$1:$G$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
   <si>
     <t>Player</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -387,6 +387,10 @@
   </si>
   <si>
     <t xml:space="preserve">Progress </t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -834,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E32B991-2ACC-47FF-BF94-29DC9CD2AFBC}">
   <dimension ref="B1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -881,7 +885,9 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>14</v>
       </c>
@@ -894,7 +900,9 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
@@ -957,7 +965,9 @@
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.4">
@@ -970,7 +980,9 @@
       <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.4">
@@ -980,7 +992,9 @@
       <c r="C12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>27</v>
       </c>
@@ -993,7 +1007,9 @@
       <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
@@ -1006,8 +1022,12 @@
       <c r="C14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
@@ -1020,7 +1040,9 @@
       <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
@@ -1033,7 +1055,9 @@
       <c r="D16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.4">
@@ -1043,8 +1067,12 @@
       <c r="C17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
+      <c r="D17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.4">
@@ -1057,7 +1085,9 @@
       <c r="D18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>83</v>
       </c>
@@ -1072,7 +1102,9 @@
       <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.4">
@@ -1085,7 +1117,9 @@
       <c r="D20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.4">
@@ -1098,7 +1132,9 @@
       <c r="D21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.4">
@@ -1108,8 +1144,12 @@
       <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.4">
@@ -1119,8 +1159,12 @@
       <c r="C23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.4">
@@ -1130,8 +1174,12 @@
       <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="D24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.4">
@@ -1144,7 +1192,9 @@
       <c r="D25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.4">
@@ -1157,7 +1207,9 @@
       <c r="D26" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.4">
@@ -1170,7 +1222,9 @@
       <c r="D27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.4">
@@ -1183,7 +1237,9 @@
       <c r="D28" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.4">
@@ -1196,7 +1252,9 @@
       <c r="D29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F29" s="1"/>
     </row>
   </sheetData>
@@ -1216,7 +1274,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1268,7 +1326,9 @@
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="I5" t="s">
         <v>13</v>
@@ -1404,7 +1464,9 @@
       <c r="D14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.4">
@@ -1417,7 +1479,9 @@
       <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.4">
@@ -1430,7 +1494,9 @@
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.4">
@@ -1443,7 +1509,9 @@
       <c r="D17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.4">
@@ -1471,7 +1539,9 @@
       <c r="D19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.4">
@@ -1499,7 +1569,9 @@
       <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.4">
@@ -1527,7 +1599,9 @@
       <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.4">
@@ -1540,7 +1614,9 @@
       <c r="D24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.4">
@@ -1568,7 +1644,9 @@
       <c r="D26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.4">
@@ -1596,7 +1674,9 @@
       <c r="D28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.4">
@@ -1624,7 +1704,9 @@
       <c r="D30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.4">
@@ -1665,7 +1747,9 @@
       <c r="D33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="2:6" ht="52.2" x14ac:dyDescent="0.4">
@@ -1678,7 +1762,9 @@
       <c r="D34" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="F34" s="1"/>
     </row>
   </sheetData>

</xml_diff>